<commit_message>
removed patents related search data
</commit_message>
<xml_diff>
--- a/src/test/test-data/WatchlistContainerTestData.xlsx
+++ b/src/test/test-data/WatchlistContainerTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bg00483545\git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="150">
   <si>
     <t>API</t>
   </si>
@@ -67,18 +72,9 @@
     <t>/wos/search</t>
   </si>
   <si>
-    <t>/patents/search</t>
-  </si>
-  <si>
     <t>?query=biology</t>
   </si>
   <si>
-    <t>/posts/search</t>
-  </si>
-  <si>
-    <t>/people/search</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -97,12 +93,6 @@
     <t>Verify that every user watchlist is private by default</t>
   </si>
   <si>
-    <t>?query=cancer&amp;size=2</t>
-  </si>
-  <si>
-    <t>?query=test post&amp;size=2</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
@@ -112,27 +102,6 @@
     <t>?itemType=wos</t>
   </si>
   <si>
-    <t>Verify that to get patents for query</t>
-  </si>
-  <si>
-    <t>OPQA-898</t>
-  </si>
-  <si>
-    <t>Verify that user is able to search for posts</t>
-  </si>
-  <si>
-    <t>OPQA-897</t>
-  </si>
-  <si>
-    <t>Verify that user is able to search for profiles</t>
-  </si>
-  <si>
-    <t>OPQA-434</t>
-  </si>
-  <si>
-    <t>?query=neon1&amp;size=1</t>
-  </si>
-  <si>
     <t>1PCONTAINER</t>
   </si>
   <si>
@@ -328,9 +297,6 @@
     <t>/container/(OPQA-3993_id)/items</t>
   </si>
   <si>
-    <t>OPQA-3993||OPQA-896||OPQA-897||OPQA-898</t>
-  </si>
-  <si>
     <t>/container/(OPQA-3993_id)/items?itemType=wos&amp;sortoption=latestupdated</t>
   </si>
   <si>
@@ -343,9 +309,6 @@
     <t>/container/(OPQA-3994_id)/items</t>
   </si>
   <si>
-    <t>OPQA-3994||OPQA-896||OPQA-897||OPQA-898</t>
-  </si>
-  <si>
     <t>OPQA-3993||OPQA-3994||OPQA-896</t>
   </si>
   <si>
@@ -463,24 +426,15 @@
     <t>status=200||contents.patents=0||contents.wos=0||contents.posts=0||contents.documents=0||contents.sse=0||contents.dra_td_sse=0||contents.ipa_sse=0||contents.total=0</t>
   </si>
   <si>
-    <t>status=200||id=(OPQA-3993_id)||type=watchlist||ispublic=true||contents.patents=2||contents.wos=2||contents.posts=2||contents.documents=0||contents.sse=0||contents.dra_td_sse=0||contents.ipa_sse=0||contents.total=6</t>
-  </si>
-  <si>
     <t>1PSEARCHV4</t>
   </si>
   <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>DEPFAIL</t>
-  </si>
-  <si>
     <t>hits[0].id||hits[1].id</t>
   </si>
   <si>
-    <t>hits[0].id</t>
-  </si>
-  <si>
     <t>{ "items" : [ {"id": "(OPQA-896_hits[0].id)", "type": "wos"}] }</t>
   </si>
   <si>
@@ -490,18 +444,9 @@
     <t>status=200||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=2</t>
   </si>
   <si>
-    <t>{"items" : [{"id": "(OPQA-896_hits[0].id)", "type": "wos"}, {"id": "(OPQA-896_hits[1].id)", "type": "wos"}, {"id": "(OPQA-898_hits[0].id)", "type": "patents"}, {"id": "(OPQA-898_hits[1].id)", "type": "patents"}, {"id": "(OPQA-897_hits[0].id)", "type": "posts"}, {"id": "(OPQA-897_hits[1].id)", "type": "posts"} ] }</t>
-  </si>
-  <si>
     <t>/container/items/contains/(OPQA-896_hits[0].id)</t>
   </si>
   <si>
-    <t>status=200||type=wos||id=(OPQA-896_hits[0].id)||||id=(OPQA-896_hits[1].id)</t>
-  </si>
-  <si>
-    <t>status=200||content_items.id=(OPQA-896_hits[0].id)||content_items.id=(OPQA-896_hits[1].id)||content_items.id=(OPQA-897_hits[0].id)||content_items.id=(OPQA-897_hits[1].id)||content_items.id=(OPQA-898_hits[0].id)||content_items.id=(OPQA-898_hits[1].id)</t>
-  </si>
-  <si>
     <t>status=200||content_items.id=(OPQA-896_hits[0].id)||content_items.id=(OPQA-896_hits[1].id)||content_items[0].type=wos</t>
   </si>
   <si>
@@ -511,15 +456,27 @@
     <t>/container/(OPQA-3994_id)/items/(OPQA-896_hits[0].id)</t>
   </si>
   <si>
-    <t/>
+    <t>{"items" : [{"id": "(OPQA-896_hits[0].id)", "type": "wos"} ] }</t>
+  </si>
+  <si>
+    <t>status=200||content_items.id=(OPQA-896_hits[0].id)||content_items.id=(OPQA-896_hits[1].id)</t>
+  </si>
+  <si>
+    <t>status=200||type=wos||id=(OPQA-896_hits[0].id)</t>
+  </si>
+  <si>
+    <t>{"items" : [{"id": "(OPQA-896_hits[1].id)", "type": "wos"}] }</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-3993_id)||type=watchlist||ispublic=true||contents.wos=2||contents.documents=0||contents.sse=0||contents.dra_td_sse=0||contents.ipa_sse=0||contents.total=2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,7 +556,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -623,9 +580,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -639,6 +593,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -685,7 +647,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -717,9 +679,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -751,6 +714,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -926,14 +890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="12.7109375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="3" width="44.85546875" collapsed="true"/>
@@ -949,7 +913,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
@@ -987,7 +951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="30">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -995,7 +959,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
@@ -1005,7 +969,7 @@
       </c>
       <c r="F2"/>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2"/>
@@ -1013,1234 +977,1135 @@
         <v>13</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="30">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>150</v>
+        <v>85</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3"/>
-      <c r="G3" s="2" t="s">
-        <v>27</v>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3"/>
       <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>153</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="K3" s="2"/>
       <c r="L3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="30">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4"/>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2"/>
       <c r="I4"/>
       <c r="J4" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>153</v>
+        <v>29</v>
       </c>
       <c r="L4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="15.75">
-      <c r="A5" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5"/>
-      <c r="G5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="2"/>
       <c r="I5"/>
       <c r="J5" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>154</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="47.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>43</v>
+        <v>101</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6"/>
+      <c r="I6" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="J6" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="300">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7"/>
-      <c r="J7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="120">
-      <c r="A8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8"/>
-      <c r="H8" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8"/>
-      <c r="J8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="300">
-      <c r="A9" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="C9" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>23</v>
+        <v>87</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G9"/>
-      <c r="H9" s="12" t="s">
-        <v>52</v>
-      </c>
+      <c r="G9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9"/>
       <c r="I9" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="105">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>23</v>
+        <v>87</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G10"/>
-      <c r="H10" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="H10"/>
       <c r="I10" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="K10"/>
       <c r="L10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="G11"/>
-      <c r="H11" s="12" t="s">
-        <v>78</v>
+      <c r="H11" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="90">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>108</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12"/>
+        <v>51</v>
+      </c>
+      <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>148</v>
+        <v>76</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="30">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>99</v>
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13" s="2" t="s">
-        <v>98</v>
+        <v>19</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" t="s">
+        <v>138</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K13"/>
+        <v>139</v>
+      </c>
+      <c r="K13" s="2"/>
       <c r="L13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14"/>
-      <c r="H14" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>98</v>
+        <v>19</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="47.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
-        <v>121</v>
+        <v>65</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>155</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>102</v>
+        <v>138</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" t="s">
-        <v>155</v>
+        <v>32</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>148</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" t="s">
-        <v>155</v>
+        <v>32</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>145</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="K18" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="K18"/>
       <c r="L18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="1" customFormat="1" ht="75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>141</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" t="s">
-        <v>155</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>124</v>
+        <v>25</v>
+      </c>
+      <c r="H19" s="12"/>
+      <c r="I19" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K19" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="K19"/>
       <c r="L19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>104</v>
+        <v>32</v>
+      </c>
+      <c r="H20" s="12"/>
+      <c r="I20" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K20" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="L20" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>109</v>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
       <c r="K21"/>
       <c r="L21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="5" t="s">
-        <v>110</v>
+      <c r="F22" s="7"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="K22"/>
       <c r="L22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="1" customFormat="1" ht="75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H23" s="13"/>
+      <c r="F23" s="7"/>
+      <c r="G23"/>
+      <c r="H23"/>
       <c r="I23" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>93</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="K23"/>
       <c r="L23" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="1" customFormat="1" ht="120">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>99</v>
+        <v>27</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24"/>
+        <v>22</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="H24"/>
       <c r="I24" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K24"/>
       <c r="L24" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="1" customFormat="1" ht="45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>99</v>
+        <v>27</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25"/>
+      <c r="F25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H25"/>
       <c r="I25" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="K25"/>
       <c r="L25" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="1" customFormat="1" ht="45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26"/>
+      <c r="F26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="H26"/>
       <c r="I26" s="2" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
       <c r="K26"/>
       <c r="L26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="1" customFormat="1" ht="180">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>99</v>
+        <v>27</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>58</v>
+        <v>22</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="H27"/>
-      <c r="I27" s="2" t="s">
-        <v>128</v>
+      <c r="I27" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>161</v>
+        <v>62</v>
       </c>
       <c r="K27"/>
       <c r="L27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="1" customFormat="1" ht="90">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28"/>
+      <c r="I28" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28"/>
-      <c r="I28" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="J28" s="2" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="K28"/>
       <c r="L28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>44</v>
+        <v>22</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="H29"/>
-      <c r="I29" s="2" t="s">
-        <v>120</v>
+      <c r="I29" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
       <c r="K29"/>
       <c r="L29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="1" customFormat="1" ht="30">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" t="s">
+        <v>138</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30"/>
-      <c r="I30" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="K30"/>
       <c r="L30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>163</v>
+        <v>49</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31"/>
-      <c r="I31" s="5" t="s">
-        <v>102</v>
+        <v>83</v>
+      </c>
+      <c r="H31" t="s">
+        <v>138</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="K31"/>
       <c r="L31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="1" customFormat="1" ht="30">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H32"/>
-      <c r="I32" s="5" t="s">
-        <v>114</v>
+        <v>22</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K32"/>
+        <v>13</v>
+      </c>
+      <c r="K32" s="2"/>
       <c r="L32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="1" customFormat="1" ht="75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H33" t="s">
-        <v>155</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="K33"/>
+      <c r="K33" s="2"/>
       <c r="L33" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="1" customFormat="1" ht="75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>21</v>
+      <c r="E34" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H34" t="s">
-        <v>155</v>
-      </c>
+      <c r="G34"/>
+      <c r="H34" s="2"/>
       <c r="I34" s="2" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="K34"/>
       <c r="L34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="30">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>29</v>
+        <v>94</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K35" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="K35"/>
       <c r="L35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="45">
-      <c r="A36" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G36"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K36" s="2"/>
-      <c r="L36" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="30">
-      <c r="A37" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K37"/>
-      <c r="L37" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="30">
-      <c r="A38" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G38"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K38"/>
-      <c r="L38" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="A3" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-898"/>
-    <hyperlink ref="A4" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-897"/>
-    <hyperlink ref="A5" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>